<commit_message>
Trabalhos desenvolvidos no dia 07-01-2019
</commit_message>
<xml_diff>
--- a/params/cmlima_substituicoes.xlsx
+++ b/params/cmlima_substituicoes.xlsx
@@ -17,9 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>buscar</t>
+  </si>
+  <si>
+    <t>padrao</t>
   </si>
   <si>
     <t>substituir_por</t>
@@ -28,7 +31,7 @@
     <t>descricao</t>
   </si>
   <si>
-    <t>padrao</t>
+    <t xml:space="preserve"> inc.</t>
   </si>
   <si>
     <t>exemplos</t>
@@ -73,6 +76,9 @@
     <t>(?&lt;=[bBcdDfgGhHjkKnpPqQtxXvVyYwWºª][lLrRsnm])\.([^0-9]{0,3}\.)*</t>
   </si>
   <si>
+    <t xml:space="preserve"> inciso </t>
+  </si>
+  <si>
     <t>(?&lt;=[bBcdDfgGhHjkKnpPqQtxXvVyYwWºª][lLrRsnm][lLrRsnm])\.([^0-9]{0,3}\.)*</t>
   </si>
   <si>
@@ -97,7 +103,16 @@
     <t>O mesmo para 2 letras: pg. fl. Mas antes, vou substituir CF.</t>
   </si>
   <si>
+    <t xml:space="preserve"> art.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> art. </t>
+  </si>
+  <si>
     <t>(?&lt;= .[^(0-9])\.</t>
+  </si>
+  <si>
+    <t>.º</t>
   </si>
   <si>
     <t>(?&lt;= [ivxlcIVXLC][ivxlcIVXLC][ivxlcIVXLC])\.</t>
@@ -110,21 +125,6 @@
   </si>
   <si>
     <t>(?&lt;= [ivxlcIVXLC][ivxlcIVXLC][ivxlcIVXLC][ivxlcIVXLC])\.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> inciso </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> art.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> art. </t>
-  </si>
-  <si>
-    <t>.º</t>
   </si>
   <si>
     <t>º</t>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t xml:space="preserve"> min.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fls.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> folhas </t>
   </si>
 </sst>
 </file>
@@ -548,10 +554,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -579,10 +585,10 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="2"/>
@@ -611,10 +617,10 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -643,7 +649,7 @@
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>36</v>
@@ -998,7 +1004,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1030,7 +1036,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1062,7 +1068,7 @@
         <v>57</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1282,8 +1288,12 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -28666,22 +28676,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -28706,20 +28716,20 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -28744,20 +28754,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -28782,20 +28792,20 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -28820,20 +28830,20 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -28858,20 +28868,20 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -28896,20 +28906,20 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -28934,18 +28944,18 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -28970,18 +28980,18 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -29006,18 +29016,18 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>

</xml_diff>